<commit_message>
review sheet wrong doc name: corrected
</commit_message>
<xml_diff>
--- a/Documents/External/ReviewRecords/Review_Sheet_CML000009 Technical Design CommLib Android.xlsx
+++ b/Documents/External/ReviewRecords/Review_Sheet_CML000009 Technical Design CommLib Android.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-4800" yWindow="-20540" windowWidth="33600" windowHeight="20540" tabRatio="904"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18960" tabRatio="904"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
@@ -87,14 +87,14 @@
     <t>Reviewer</t>
   </si>
   <si>
-    <t>Document: CML000009 CommLib API Android
-Product/Platform: CommLib Android/CDP2 Platform</t>
-  </si>
-  <si>
     <t>Bas Flaton</t>
   </si>
   <si>
     <t>No comments</t>
+  </si>
+  <si>
+    <t>Document: CML000009 Technical Design CommLib Android
+Product/Platform: CommLib Android/CDP2 Platform</t>
   </si>
 </sst>
 </file>
@@ -987,7 +987,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="80" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:H5"/>
+      <selection activeCell="A6" sqref="A6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="6" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="34" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
@@ -1241,10 +1241,10 @@
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="23"/>

</xml_diff>

<commit_message>
Fixed mentioning wrong component name in Technical Documentation
</commit_message>
<xml_diff>
--- a/Documents/External/ReviewRecords/Review_Sheet_CML000009 Technical Design CommLib Android.xlsx
+++ b/Documents/External/ReviewRecords/Review_Sheet_CML000009 Technical Design CommLib Android.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27011"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/310088528p/dev/android-commlib-workspace/Source/commlib/Documents/External/ReviewRecords/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/310246817/Documents/git/dicomm-android/Documents/External/ReviewRecords/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18960" tabRatio="904"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18960" tabRatio="904" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Purpose</t>
   </si>
@@ -95,6 +95,9 @@
   <si>
     <t>Document: CML000009 Technical Design CommLib Android
 Product/Platform: CommLib Android/CDP2 Platform</t>
+  </si>
+  <si>
+    <t>Marco Pace</t>
   </si>
 </sst>
 </file>
@@ -986,8 +989,8 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="80" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:H6"/>
+    <sheetView view="pageLayout" zoomScale="80" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1167,7 +1170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" zoomScale="80" workbookViewId="0">
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScale="80" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1251,11 +1254,15 @@
       <c r="G6" s="24"/>
       <c r="H6" s="25"/>
     </row>
-    <row r="7" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" customFormat="1" ht="26" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
+      <c r="C7" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>17</v>
+      </c>
       <c r="E7" s="18"/>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>

</xml_diff>